<commit_message>
Lots of writing, analysis, cleanup
</commit_message>
<xml_diff>
--- a/files/SFModelTable.xlsx
+++ b/files/SFModelTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dan\_Remote_projects\ccp-sROS\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BEAFF6-073E-4676-A38B-1BB8DA0852D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09481325-A1FD-41C0-B1D5-0E2795E65A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{283E095B-EF87-443F-89B7-5C13059C1829}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Model</t>
   </si>
@@ -47,12 +47,6 @@
     <t>axb mod</t>
   </si>
   <si>
-    <t>R^2</t>
-  </si>
-  <si>
-    <t>Dataset</t>
-  </si>
-  <si>
     <t>All SF in FBP database, incl. deciduous</t>
   </si>
   <si>
@@ -78,14 +72,144 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>cr_isi</t>
+  </si>
+  <si>
+    <t>cr_isim</t>
+  </si>
+  <si>
+    <t>ISI2SFC</t>
+  </si>
+  <si>
+    <t>ISIm2SFC</t>
+  </si>
+  <si>
+    <t>AIC</t>
+  </si>
+  <si>
+    <t>BIC</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>Modified SF (all SF, modified PPDF)</t>
+  </si>
+  <si>
+    <t>sf.axb.isi.mod</t>
+  </si>
+  <si>
+    <t>Conifer SF excluding PPDF</t>
+  </si>
+  <si>
+    <t>con.lm.mod</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P-R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>MEA</t>
+  </si>
+  <si>
+    <t>sros.st</t>
+  </si>
+  <si>
+    <t>sros.isi2.mod</t>
+  </si>
+  <si>
+    <t>ISI^2</t>
+  </si>
+  <si>
+    <t>FBP C6S</t>
+  </si>
+  <si>
+    <t>CR (a=30)</t>
+  </si>
+  <si>
+    <t>VW C4S</t>
+  </si>
+  <si>
+    <t>VW C3S</t>
+  </si>
+  <si>
+    <t>CR (a=20)</t>
+  </si>
+  <si>
+    <t>CR (a=15)</t>
+  </si>
+  <si>
+    <t>Source Data</t>
+  </si>
+  <si>
+    <t>Visual inspection, simple structure stands (VW 1989, FCFDG 1992)</t>
+  </si>
+  <si>
+    <t>Visual inspection, mature pine stands (VW 1993)</t>
+  </si>
+  <si>
+    <t>Visual inspection, immature pine stands (VW 1993)</t>
+  </si>
+  <si>
+    <t>FBP D1</t>
+  </si>
+  <si>
+    <t>c6s</t>
+  </si>
+  <si>
+    <t>sf.vw93i</t>
+  </si>
+  <si>
+    <t>sf.vw93m</t>
+  </si>
+  <si>
+    <t>r name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -133,9 +257,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -173,7 +297,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -279,7 +403,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -421,7 +545,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -429,76 +553,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6D5552-DEFD-45E3-88F0-AEC817569D00}">
-  <dimension ref="B2:F6"/>
+  <dimension ref="A2:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="31.88671875" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="45.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>0.69</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>0.57240000000000002</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>0.19800000000000001</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>2</v>
+      <c r="D13">
+        <v>0.7601</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>0.78739999999999999</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>